<commit_message>
Jozam UI concept with Qt Designer
</commit_message>
<xml_diff>
--- a/EDT.xlsx
+++ b/EDT.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion lastEdited="4" lowestEdited="4" rupBuild="3820"/>
-  <workbookPr date1904="0"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="153222"/>
   <bookViews>
-    <workbookView activeTab="2"/>
+    <workbookView visibility="hidden" xWindow="0" yWindow="0" windowWidth="24000" windowHeight="11865" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Analyse" sheetId="1" r:id="rId1"/>
@@ -14,102 +14,25 @@
     <sheet name="Tasks(S2)" sheetId="5" r:id="rId5"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlnm.Sheet_Title" localSheetId="0">"Analyse"</definedName>
+    <definedName name="_xlnm.Sheet_Title" localSheetId="1">"Conges"</definedName>
+    <definedName name="_xlnm.Sheet_Title" localSheetId="2">"Tasks"</definedName>
+    <definedName name="_xlnm.Sheet_Title" localSheetId="4">"Tasks(S2)"</definedName>
+    <definedName name="_xlnm.Sheet_Title" localSheetId="3">"Tasks(S3)"</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="0">#REF!</definedName>
-    <definedName name="_xlnm.Sheet_Title" localSheetId="0">"Analyse"</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="1">#REF!</definedName>
-    <definedName name="_xlnm.Sheet_Title" localSheetId="1">"Conges"</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="2">#REF!</definedName>
-    <definedName name="_xlnm.Sheet_Title" localSheetId="2">"Tasks"</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="4">#REF!</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="3">#REF!</definedName>
-    <definedName name="_xlnm.Sheet_Title" localSheetId="3">"Tasks(S3)"</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="4">#REF!</definedName>
-    <definedName name="_xlnm.Sheet_Title" localSheetId="4">"Tasks(S2)"</definedName>
   </definedNames>
-  <calcPr calcMode="auto" iterate="1" iterateCount="100" iterateDelta="0.001"/>
-  <webPublishing allowPng="1" css="0" characterSet="UTF-8"/>
+  <calcPr calcId="152511" iterate="1"/>
+  <oleSize ref="A1"/>
+  <webPublishing css="0" allowPng="1" codePage="0"/>
 </workbook>
 </file>
 
-<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <authors>
-    <author>Marc Boyer</author>
-  </authors>
-  <commentList>
-    <comment ref="B51" authorId="0">
-      <text>
-        <t>05.61.21.68.69</t>
-      </text>
-    </comment>
-    <comment ref="B5" authorId="0">
-      <text>
-        <t>Modèle CPL analytique possible car au + 4 inputs, en s'inspirant des travaux ShapedStair</t>
-      </text>
-    </comment>
-    <comment ref="V10" authorId="0">
-      <text>
-        <t>Decoupage trames: creer nvx VL
-Frame abort: VL en rab + analmyse séparée suivantr priorités</t>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
-<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <authors>
-    <author>Marc Boyer</author>
-  </authors>
-  <commentList>
-    <comment ref="B51" authorId="0">
-      <text>
-        <t>05.61.21.68.69</t>
-      </text>
-    </comment>
-    <comment ref="B4" authorId="0">
-      <text>
-        <t>Modèle CPL analytique possible car au + 4 inputs, en s'inspirant des travaux ShapedStair</t>
-      </text>
-    </comment>
-    <comment ref="V10" authorId="0">
-      <text>
-        <t>Decoupage trames: creer nvx VL
-Frame abort: VL en rab + analmyse séparée suivantr priorités</t>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
-<file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <authors>
-    <author>Marc Boyer</author>
-  </authors>
-  <commentList>
-    <comment ref="B49" authorId="0">
-      <text>
-        <t>05.61.21.68.69</t>
-      </text>
-    </comment>
-    <comment ref="B7" authorId="0">
-      <text>
-        <t>Modèle CPL analytique possible car au + 4 inputs, en s'inspirant des travaux ShapedStair</t>
-      </text>
-    </comment>
-    <comment ref="V10" authorId="0">
-      <text>
-        <t>Decoupage trames: creer nvx VL
-Frame abort: VL en rab + analmyse séparée suivantr priorités</t>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="104" count="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="382" uniqueCount="140">
   <si>
     <t>RTNS</t>
   </si>
@@ -168,9 +91,6 @@
     <t>Chap 7: packets</t>
   </si>
   <si>
-    <t/>
-  </si>
-  <si>
     <t>Partie théorique</t>
   </si>
   <si>
@@ -405,9 +325,6 @@
     <t>Tel Nicolas/Jorn</t>
   </si>
   <si>
-    <t>X</t>
-  </si>
-  <si>
     <t>Faire le RT</t>
   </si>
   <si>
@@ -421,55 +338,157 @@
   </si>
   <si>
     <t>Licence RTaW</t>
+  </si>
+  <si>
+    <t>R2</t>
+  </si>
+  <si>
+    <t>Congés</t>
+  </si>
+  <si>
+    <t>Vacances Ski</t>
+  </si>
+  <si>
+    <t>Toussain</t>
+  </si>
+  <si>
+    <t>Pont</t>
+  </si>
+  <si>
+    <t>Eval analytique -&gt; Doose</t>
+  </si>
+  <si>
+    <t>Notes Pierre</t>
+  </si>
+  <si>
+    <t>Divers</t>
+  </si>
+  <si>
+    <t>Conflit EDT 6/2/15</t>
+  </si>
+  <si>
+    <t>Finir modifs</t>
+  </si>
+  <si>
+    <t>Relance manu EDT</t>
+  </si>
+  <si>
+    <t>Task-Manager</t>
+  </si>
+  <si>
+    <t>Faire</t>
+  </si>
+  <si>
+    <t>Spécification</t>
+  </si>
+  <si>
+    <t>RdV</t>
+  </si>
+  <si>
+    <t>Programme conf-call</t>
+  </si>
+  <si>
+    <t>Réponse DBLP</t>
+  </si>
+  <si>
+    <t>Manu: conflit EDT</t>
+  </si>
+  <si>
+    <t>Tel MAIF voiture</t>
+  </si>
+  <si>
+    <t>Tel karim Portet</t>
+  </si>
+  <si>
+    <t>Imprimer doc MAJ Duco</t>
+  </si>
+  <si>
+    <t>Point Eric</t>
+  </si>
+  <si>
+    <t>Organiser réunion Airbus</t>
+  </si>
+  <si>
+    <t>Fred: co-tutelle Barcelone</t>
+  </si>
+  <si>
+    <t>Répondre Barberis</t>
+  </si>
+  <si>
+    <t>HP15</t>
+  </si>
+  <si>
+    <t>Bilan</t>
+  </si>
+  <si>
+    <t>Transfert</t>
+  </si>
+  <si>
+    <t>Surveiller svn</t>
+  </si>
+  <si>
+    <t>Relire</t>
+  </si>
+  <si>
+    <t>Voir EDT</t>
+  </si>
+  <si>
+    <t>Répondre sécu Carlos</t>
+  </si>
+  <si>
+    <t>relance Eric/Lachaize/Xentium/Recore</t>
+  </si>
+  <si>
+    <t>Répondre Lyne</t>
+  </si>
+  <si>
+    <t>mail Kalray</t>
+  </si>
+  <si>
+    <t>EasyChair</t>
+  </si>
+  <si>
+    <t>Tel médecin</t>
+  </si>
+  <si>
+    <t>Tel ophtalmo</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
-    <numFmt formatCode="dddd dd mmm yy" numFmtId="100"/>
-    <numFmt formatCode="dd/mm" numFmtId="101"/>
+    <numFmt numFmtId="164" formatCode="dddd\ dd\ mmm\ yy"/>
+    <numFmt numFmtId="165" formatCode="dd/mm"/>
   </numFmts>
   <fonts count="5">
     <font>
-      <b val="0"/>
-      <i val="0"/>
+      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Sans"/>
-      <strike val="0"/>
     </font>
     <font>
-      <b val="0"/>
-      <i val="0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Sans"/>
-      <sz val="10"/>
-      <strike val="0"/>
     </font>
     <font>
-      <b val="0"/>
-      <i val="0"/>
+      <sz val="8"/>
       <color rgb="FF000000"/>
       <name val="Sans"/>
-      <sz val="8"/>
-      <strike val="0"/>
     </font>
     <font>
-      <b val="1"/>
-      <i val="0"/>
+      <b/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Sans"/>
-      <sz val="10"/>
-      <strike val="0"/>
     </font>
     <font>
-      <b val="0"/>
-      <i val="0"/>
+      <strike/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Sans"/>
-      <sz val="10"/>
-      <strike val="1"/>
     </font>
   </fonts>
   <fills count="6">
@@ -501,338 +520,539 @@
     </fill>
   </fills>
   <borders count="2">
-    <border diagonalUp="0" diagonalDown="0">
-      <start style="none">
-        <color rgb="FFC7C7C7"/>
-      </start>
-      <end style="none">
-        <color rgb="FFC7C7C7"/>
-      </end>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
     </border>
-    <border diagonalUp="0" diagonalDown="0">
-      <start style="none">
-        <color rgb="FFC7C7C7"/>
-      </start>
-      <end style="none">
-        <color rgb="FFC7C7C7"/>
-      </end>
-      <top style="none">
-        <color rgb="FFC7C7C7"/>
-      </top>
-      <bottom style="none">
-        <color rgb="FFC7C7C7"/>
-      </bottom>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="94">
-    <xf applyAlignment="0" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="1" fillId="0" borderId="1" numFmtId="0" xfId="0">
-      <alignment horizontal="general" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="1" fillId="0" borderId="1" numFmtId="0" xfId="0">
-      <alignment horizontal="general" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="1" fillId="0" borderId="1" numFmtId="100" xfId="0">
-      <alignment horizontal="general" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="1" fillId="0" borderId="1" numFmtId="0" xfId="0">
-      <alignment horizontal="center" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="1" fillId="0" borderId="1" numFmtId="0" xfId="0">
-      <alignment horizontal="general" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="2" fillId="0" borderId="1" numFmtId="101" xfId="0">
-      <alignment horizontal="center" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="2" fillId="0" borderId="1" numFmtId="101" xfId="0">
-      <alignment horizontal="general" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="3" fillId="2" borderId="1" numFmtId="0" xfId="0">
-      <alignment horizontal="center" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="1" fillId="3" borderId="1" numFmtId="0" xfId="0">
-      <alignment horizontal="general" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="1" fillId="0" borderId="1" numFmtId="0" xfId="0">
-      <alignment horizontal="center" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="1" fillId="0" borderId="1" numFmtId="0" xfId="0">
-      <alignment horizontal="center" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="1" fillId="0" borderId="1" numFmtId="0" xfId="0">
-      <alignment horizontal="general" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="4" fillId="0" borderId="1" numFmtId="0" xfId="0">
-      <alignment horizontal="general" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="1" fillId="0" borderId="1" numFmtId="0" xfId="0">
-      <alignment horizontal="center" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="1" fillId="0" borderId="1" numFmtId="0" xfId="0">
-      <alignment horizontal="center" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="1" fillId="0" borderId="1" numFmtId="0" xfId="0">
-      <alignment horizontal="center" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="1" fillId="0" borderId="1" numFmtId="0" xfId="0">
-      <alignment horizontal="general" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="1" fillId="0" borderId="1" numFmtId="0" xfId="0">
-      <alignment horizontal="center" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="1" fillId="0" borderId="1" numFmtId="0" xfId="0">
-      <alignment horizontal="center" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="1" fillId="0" borderId="1" numFmtId="0" xfId="0">
-      <alignment horizontal="general" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="1" fillId="0" borderId="1" numFmtId="0" xfId="0">
-      <alignment horizontal="center" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="1" fillId="0" borderId="1" numFmtId="0" xfId="0">
-      <alignment horizontal="center" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="1" fillId="4" borderId="1" numFmtId="0" xfId="0">
-      <alignment horizontal="general" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="1" fillId="0" borderId="1" numFmtId="0" xfId="0">
-      <alignment horizontal="center" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="1" fillId="0" borderId="1" numFmtId="0" xfId="0">
-      <alignment horizontal="center" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="1" fillId="0" borderId="1" numFmtId="0" xfId="0">
-      <alignment horizontal="center" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="1" fillId="0" borderId="1" numFmtId="0" xfId="0">
-      <alignment horizontal="general" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="3" fillId="5" borderId="1" numFmtId="0" xfId="0">
-      <alignment horizontal="center" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="1" fillId="0" borderId="1" numFmtId="0" xfId="0">
-      <alignment horizontal="left" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="1" fillId="0" borderId="1" numFmtId="0" xfId="0">
-      <alignment horizontal="center" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="1" fillId="0" borderId="1" numFmtId="0" xfId="0">
-      <alignment horizontal="center" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="1" fillId="0" borderId="1" numFmtId="0" xfId="0">
-      <alignment horizontal="center" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="1" fillId="0" borderId="1" numFmtId="0" xfId="0">
-      <alignment horizontal="center" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="1" fillId="0" borderId="1" numFmtId="0" xfId="0">
-      <alignment horizontal="center" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="1" fillId="0" borderId="1" numFmtId="0" xfId="0">
-      <alignment horizontal="general" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="2" fillId="0" borderId="1" numFmtId="101" xfId="0">
-      <alignment horizontal="center" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="2" fillId="0" borderId="1" numFmtId="101" xfId="0">
-      <alignment horizontal="general" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="3" fillId="2" borderId="1" numFmtId="0" xfId="0">
-      <alignment horizontal="center" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="4" fillId="0" borderId="1" numFmtId="0" xfId="0">
-      <alignment horizontal="general" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="1" fillId="3" borderId="1" numFmtId="0" xfId="0">
-      <alignment horizontal="general" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="1" fillId="0" borderId="1" numFmtId="0" xfId="0">
-      <alignment horizontal="center" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="1" fillId="0" borderId="1" numFmtId="0" xfId="0">
-      <alignment horizontal="center" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="1" fillId="0" borderId="1" numFmtId="0" xfId="0">
-      <alignment horizontal="general" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="1" fillId="0" borderId="1" numFmtId="0" xfId="0">
-      <alignment horizontal="center" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="1" fillId="0" borderId="1" numFmtId="0" xfId="0">
-      <alignment horizontal="center" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="1" fillId="0" borderId="1" numFmtId="0" xfId="0">
-      <alignment horizontal="center" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="1" fillId="0" borderId="1" numFmtId="0" xfId="0">
-      <alignment horizontal="general" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="1" fillId="0" borderId="1" numFmtId="0" xfId="0">
-      <alignment horizontal="center" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="1" fillId="0" borderId="1" numFmtId="0" xfId="0">
-      <alignment horizontal="center" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="1" fillId="0" borderId="1" numFmtId="0" xfId="0">
-      <alignment horizontal="general" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="1" fillId="0" borderId="1" numFmtId="0" xfId="0">
-      <alignment horizontal="center" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="1" fillId="0" borderId="1" numFmtId="0" xfId="0">
-      <alignment horizontal="center" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="1" fillId="4" borderId="1" numFmtId="0" xfId="0">
-      <alignment horizontal="general" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="1" fillId="0" borderId="1" numFmtId="0" xfId="0">
-      <alignment horizontal="center" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="1" fillId="0" borderId="1" numFmtId="0" xfId="0">
-      <alignment horizontal="center" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="1" fillId="0" borderId="1" numFmtId="0" xfId="0">
-      <alignment horizontal="center" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="1" fillId="0" borderId="1" numFmtId="0" xfId="0">
-      <alignment horizontal="general" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="3" fillId="5" borderId="1" numFmtId="0" xfId="0">
-      <alignment horizontal="center" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="1" fillId="0" borderId="1" numFmtId="0" xfId="0">
-      <alignment horizontal="left" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="1" fillId="0" borderId="1" numFmtId="0" xfId="0">
-      <alignment horizontal="center" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="1" fillId="0" borderId="1" numFmtId="0" xfId="0">
-      <alignment horizontal="center" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="1" fillId="0" borderId="1" numFmtId="0" xfId="0">
-      <alignment horizontal="center" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="1" fillId="0" borderId="1" numFmtId="0" xfId="0">
-      <alignment horizontal="center" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="1" fillId="0" borderId="1" numFmtId="0" xfId="0">
-      <alignment horizontal="center" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="1" fillId="0" borderId="1" numFmtId="0" xfId="0">
-      <alignment horizontal="general" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="2" fillId="0" borderId="1" numFmtId="101" xfId="0">
-      <alignment horizontal="center" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="2" fillId="0" borderId="1" numFmtId="101" xfId="0">
-      <alignment horizontal="general" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="4" fillId="2" borderId="1" numFmtId="0" xfId="0">
-      <alignment horizontal="center" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="3" fillId="2" borderId="1" numFmtId="0" xfId="0">
-      <alignment horizontal="center" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="4" fillId="0" borderId="1" numFmtId="0" xfId="0">
-      <alignment horizontal="general" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="1" fillId="3" borderId="1" numFmtId="0" xfId="0">
-      <alignment horizontal="general" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="1" fillId="0" borderId="1" numFmtId="0" xfId="0">
-      <alignment horizontal="center" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="4" fillId="0" borderId="1" numFmtId="0" xfId="0">
-      <alignment horizontal="general" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="1" fillId="0" borderId="1" numFmtId="0" xfId="0">
-      <alignment horizontal="center" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="1" fillId="0" borderId="1" numFmtId="0" xfId="0">
-      <alignment horizontal="general" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="1" fillId="0" borderId="1" numFmtId="0" xfId="0">
-      <alignment horizontal="center" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="1" fillId="0" borderId="1" numFmtId="0" xfId="0">
-      <alignment horizontal="center" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="1" fillId="0" borderId="1" numFmtId="0" xfId="0">
-      <alignment horizontal="center" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="1" fillId="0" borderId="1" numFmtId="0" xfId="0">
-      <alignment horizontal="general" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="1" fillId="0" borderId="1" numFmtId="0" xfId="0">
-      <alignment horizontal="center" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="1" fillId="0" borderId="1" numFmtId="0" xfId="0">
-      <alignment horizontal="center" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="1" fillId="0" borderId="1" numFmtId="0" xfId="0">
-      <alignment horizontal="general" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="1" fillId="0" borderId="1" numFmtId="0" xfId="0">
-      <alignment horizontal="center" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="1" fillId="0" borderId="1" numFmtId="0" xfId="0">
-      <alignment horizontal="center" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="1" fillId="0" borderId="1" numFmtId="0" xfId="0">
-      <alignment horizontal="center" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="1" fillId="0" borderId="1" numFmtId="0" xfId="0">
-      <alignment horizontal="center" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="1" fillId="0" borderId="1" numFmtId="0" xfId="0">
-      <alignment horizontal="center" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="1" fillId="0" borderId="1" numFmtId="0" xfId="0">
-      <alignment horizontal="general" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="3" fillId="5" borderId="1" numFmtId="0" xfId="0">
-      <alignment horizontal="center" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="1" fillId="0" borderId="1" numFmtId="0" xfId="0">
-      <alignment horizontal="center" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="1" fillId="0" borderId="1" numFmtId="0" xfId="0">
-      <alignment horizontal="center" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="1" fillId="0" borderId="1" numFmtId="0" xfId="0">
-      <alignment horizontal="center" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="1" fillId="0" borderId="1" numFmtId="0" xfId="0">
-      <alignment horizontal="center" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
+  <cellStyles count="1">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+  </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="44546A"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E7E6E6"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="5B9BD5"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="ED7D31"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="A5A5A5"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="FFC000"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4472C4"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="70AD47"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0563C1"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="954F72"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr>
-    <pageSetUpPr fitToPage="0"/>
-  </sheetPr>
-  <dimension ref="A2:B2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:IV2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" style="1" width="11.99928" customWidth="1"/>
-    <col min="2" max="2" style="1" width="9.142308"/>
-    <col min="3" max="256" style="1"/>
+    <col min="1" max="1" width="12" style="1" customWidth="1"/>
+    <col min="2" max="2" width="9.125" style="1"/>
+    <col min="3" max="256" width="0" style="1" hidden="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:2">
-      <c r="A2" t="str">
-        <v>R2</v>
+      <c r="A2" t="s">
+        <v>102</v>
       </c>
       <c r="B2" t="e">
         <f>COUNTIF(#REF!,"*R2*")</f>
@@ -841,42 +1061,38 @@
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" selectLockedCells="1" sort="0" autoFilter="0" pivotTables="0" selectUnlockedCells="1"/>
-  <printOptions/>
   <pageMargins left="1" right="1" top="1.667" bottom="1.667" header="1" footer="1"/>
-  <pageSetup blackAndWhite="0" cellComments="asDisplayed" draft="0" errors="displayed" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="0"/>
+  <pageSetup paperSize="9" orientation="portrait" cellComments="asDisplayed"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr>
-    <pageSetUpPr fitToPage="0"/>
-  </sheetPr>
-  <dimension ref="A1:C29"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:IV29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" style="2" width="22.132" customWidth="1"/>
-    <col min="2" max="2" style="2" width="7.285276" customWidth="1"/>
-    <col min="3" max="3" style="2" width="12.85637" bestFit="1" customWidth="1"/>
-    <col min="4" max="256" style="2"/>
+    <col min="1" max="1" width="22.125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="7.25" style="2" customWidth="1"/>
+    <col min="3" max="3" width="12.875" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="256" width="0" style="2" hidden="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="C1" t="str">
-        <v>Congés</v>
+      <c r="C1" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="3">
         <v>41701</v>
       </c>
-      <c r="C3" t="str">
-        <v>Vacances Ski</v>
+      <c r="C3" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -936,8 +1152,8 @@
       <c r="A17" s="3">
         <v>41932</v>
       </c>
-      <c r="C17" t="str">
-        <v>Toussain</v>
+      <c r="C17" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="18" spans="1:3">
@@ -989,8 +1205,8 @@
       <c r="A28" s="3">
         <v>41953</v>
       </c>
-      <c r="C28" t="str">
-        <v>Pont</v>
+      <c r="C28" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="29" spans="1:3">
@@ -1003,46 +1219,42 @@
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" selectLockedCells="1" sort="0" autoFilter="0" pivotTables="0" selectUnlockedCells="1"/>
-  <printOptions/>
   <pageMargins left="1" right="1" top="1.667" bottom="1.667" header="1" footer="1"/>
-  <pageSetup blackAndWhite="0" cellComments="asDisplayed" draft="0" errors="displayed" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="0"/>
+  <pageSetup paperSize="9" orientation="portrait" cellComments="asDisplayed"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr>
-    <pageSetUpPr fitToPage="0"/>
-  </sheetPr>
-  <dimension ref="A1:X65536"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:IV65536"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="1">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" style="4" width="2.856971" customWidth="1"/>
-    <col min="2" max="2" style="5" width="24.28425" customWidth="1"/>
-    <col min="3" max="3" style="6" width="5.285397" hidden="1" customWidth="1"/>
-    <col min="4" max="4" style="4" width="4.285457" customWidth="1"/>
-    <col min="5" max="5" style="5" width="4.285457" customWidth="1"/>
-    <col min="6" max="6" style="5" width="2.856971" customWidth="1"/>
-    <col min="7" max="7" style="5" width="24.28425" customWidth="1"/>
-    <col min="8" max="8" style="5" width="5.285397" hidden="1" customWidth="1"/>
-    <col min="9" max="10" style="5" width="4.285457" customWidth="1"/>
-    <col min="11" max="11" style="5" width="2.856971" customWidth="1"/>
-    <col min="12" max="12" style="5" width="24.28425" customWidth="1"/>
-    <col min="13" max="13" style="5" width="5.285397" hidden="1" customWidth="1"/>
-    <col min="14" max="15" style="5" width="4.285457" customWidth="1"/>
-    <col min="16" max="16" style="5" width="2.856971" customWidth="1"/>
-    <col min="17" max="17" style="5" width="24.28425" customWidth="1"/>
-    <col min="18" max="18" style="7" width="5.285397" hidden="1" customWidth="1"/>
-    <col min="19" max="20" style="5" width="4.285457" customWidth="1"/>
-    <col min="21" max="21" style="5" width="2.856971" customWidth="1"/>
-    <col min="22" max="22" style="5" width="24.28425" customWidth="1"/>
-    <col min="23" max="24" style="5" width="9.142308"/>
-    <col min="25" max="256" style="5"/>
+    <col min="1" max="1" width="2.875" style="4" customWidth="1"/>
+    <col min="2" max="2" width="24.25" style="5" customWidth="1"/>
+    <col min="3" max="3" width="5.25" style="6" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="4.25" style="4" customWidth="1"/>
+    <col min="5" max="5" width="4.25" style="5" customWidth="1"/>
+    <col min="6" max="6" width="2.875" style="5" customWidth="1"/>
+    <col min="7" max="7" width="24.25" style="5" customWidth="1"/>
+    <col min="8" max="8" width="5.25" style="5" hidden="1" customWidth="1"/>
+    <col min="9" max="10" width="4.25" style="5" customWidth="1"/>
+    <col min="11" max="11" width="2.875" style="5" customWidth="1"/>
+    <col min="12" max="12" width="24.25" style="5" customWidth="1"/>
+    <col min="13" max="13" width="5.25" style="5" hidden="1" customWidth="1"/>
+    <col min="14" max="15" width="4.25" style="5" customWidth="1"/>
+    <col min="16" max="16" width="2.875" style="5" customWidth="1"/>
+    <col min="17" max="17" width="24.25" style="5" customWidth="1"/>
+    <col min="18" max="18" width="5.25" style="7" hidden="1" customWidth="1"/>
+    <col min="19" max="20" width="4.25" style="5" customWidth="1"/>
+    <col min="21" max="21" width="2.875" style="5" customWidth="1"/>
+    <col min="22" max="22" width="24.25" style="5" customWidth="1"/>
+    <col min="23" max="24" width="9.125" style="5"/>
+    <col min="25" max="256" width="0" style="5" hidden="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:24">
@@ -1093,11 +1305,11 @@
         <v>41759</v>
       </c>
       <c r="I2" s="10">
-        <f>IF(ISBLANK(H2),"",NETWORKDAYS(TODAY(),H2,Conges!$B:$B))</f>
-        <v>192</v>
-      </c>
-      <c r="L2" t="str">
-        <v>Eval analytique -&gt; Doose</v>
+        <f ca="1">IF(ISBLANK(H2),"",NETWORKDAYS(TODAY(),H2,Conges!$B:$B))</f>
+        <v>-208</v>
+      </c>
+      <c r="L2" t="s">
+        <v>107</v>
       </c>
       <c r="Q2" s="9" t="s">
         <v>11</v>
@@ -1138,87 +1350,87 @@
         <v>18</v>
       </c>
       <c r="H4" s="6"/>
-      <c r="I4" s="10" t="s">
-        <f>IF(ISBLANK(H4),"",NETWORKDAYS(TODAY(),H4,Conges!$B:$B))</f>
-        <v>19</v>
+      <c r="I4" s="10" t="str">
+        <f ca="1">IF(ISBLANK(H4),"",NETWORKDAYS(TODAY(),H4,Conges!$B:$B))</f>
+        <v/>
       </c>
       <c r="L4" s="13"/>
       <c r="R4" s="5"/>
       <c r="V4" s="12" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="W4" s="7"/>
     </row>
     <row r="5" spans="1:24">
       <c r="B5" t="s">
+        <v>20</v>
+      </c>
+      <c r="G5" t="s">
         <v>21</v>
       </c>
-      <c r="G5" t="s">
-        <v>22</v>
-      </c>
       <c r="H5" s="6"/>
-      <c r="I5" s="10" t="s">
-        <f>IF(ISBLANK(H5),"",NETWORKDAYS(TODAY(),H5,Conges!$A:$A))</f>
-        <v>19</v>
+      <c r="I5" s="10" t="str">
+        <f ca="1">IF(ISBLANK(H5),"",NETWORKDAYS(TODAY(),H5,Conges!$A:$A))</f>
+        <v/>
       </c>
       <c r="L5" s="13"/>
       <c r="R5" s="5"/>
       <c r="V5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="W5" s="7"/>
     </row>
     <row r="6" spans="1:24">
       <c r="B6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D6" s="14"/>
       <c r="G6" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q6" s="9" t="s">
         <v>25</v>
-      </c>
-      <c r="Q6" s="9" t="s">
-        <v>26</v>
       </c>
       <c r="R6" s="5"/>
       <c r="V6" t="s">
+        <v>26</v>
+      </c>
+      <c r="W6" s="7"/>
+    </row>
+    <row r="7" spans="1:24">
+      <c r="D7" s="15" t="str">
+        <f ca="1">IF(ISBLANK(C7),"",NETWORKDAYS(TODAY(),C7,Conges!$B:$B))</f>
+        <v/>
+      </c>
+      <c r="G7" t="s">
         <v>27</v>
-      </c>
-      <c r="W6" s="7"/>
-    </row>
-    <row r="7" spans="1:24">
-      <c r="D7" s="15" t="s">
-        <f>IF(ISBLANK(C7),"",NETWORKDAYS(TODAY(),C7,Conges!$B:$B))</f>
-        <v>19</v>
-      </c>
-      <c r="G7" t="s">
-        <v>28</v>
       </c>
       <c r="H7" s="6"/>
       <c r="L7" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q7" t="s">
         <v>29</v>
-      </c>
-      <c r="Q7" t="s">
-        <v>30</v>
       </c>
       <c r="R7" s="5"/>
       <c r="W7" s="7"/>
     </row>
     <row r="8" spans="1:24">
       <c r="D8" s="5"/>
-      <c r="G8" s="13" t="str">
-        <v>Notes Pierre</v>
+      <c r="G8" s="13" t="s">
+        <v>108</v>
       </c>
       <c r="H8" s="7"/>
       <c r="L8" s="13"/>
       <c r="R8" s="5"/>
       <c r="V8" s="9" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="W8" s="7"/>
     </row>
     <row r="9" spans="1:24">
-      <c r="B9" s="8" t="str">
-        <v>Divers</v>
+      <c r="B9" s="8" t="s">
+        <v>109</v>
       </c>
       <c r="D9" s="5"/>
       <c r="F9" s="4"/>
@@ -1226,28 +1438,28 @@
       <c r="I9" s="16"/>
       <c r="M9" s="7"/>
       <c r="Q9" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="R9" s="5"/>
       <c r="V9" s="17" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="W9" s="7"/>
     </row>
     <row r="10" spans="1:24">
-      <c r="B10" t="str">
-        <v>Conflit EDT 6/2/15</v>
+      <c r="B10" t="s">
+        <v>110</v>
       </c>
       <c r="D10" s="5"/>
       <c r="F10" s="4"/>
       <c r="L10" s="13"/>
       <c r="M10" s="6"/>
       <c r="Q10" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="R10" s="5"/>
       <c r="V10" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="W10" s="7"/>
     </row>
@@ -1257,11 +1469,11 @@
       <c r="D11" s="5"/>
       <c r="F11" s="4"/>
       <c r="Q11" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="R11" s="5"/>
       <c r="V11" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="W11" s="7"/>
     </row>
@@ -1271,110 +1483,110 @@
       <c r="D12" s="5"/>
       <c r="F12" s="4"/>
       <c r="G12" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H12" s="6"/>
       <c r="I12" s="18"/>
       <c r="L12" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q12" t="s">
         <v>36</v>
-      </c>
-      <c r="Q12" t="s">
-        <v>37</v>
       </c>
       <c r="R12" s="5"/>
       <c r="V12" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="W12" s="7">
         <v>41817</v>
       </c>
       <c r="X12" s="19">
-        <f>IF(ISBLANK(W12),"",NETWORKDAYS(TODAY(),W12,Conges!$B:$B))</f>
-        <v>150</v>
+        <f ca="1">IF(ISBLANK(W12),"",NETWORKDAYS(TODAY(),W12,Conges!$B:$B))</f>
+        <v>-166</v>
       </c>
     </row>
     <row r="13" spans="1:24">
       <c r="B13" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D13" s="5"/>
       <c r="G13" t="s">
+        <v>39</v>
+      </c>
+      <c r="L13" t="s">
         <v>40</v>
       </c>
-      <c r="L13" t="s">
+      <c r="Q13" s="20" t="s">
         <v>41</v>
-      </c>
-      <c r="Q13" s="20" t="s">
-        <v>42</v>
       </c>
       <c r="R13" s="5"/>
       <c r="V13" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="W13" s="7"/>
-      <c r="X13" s="19" t="s">
-        <f>IF(ISBLANK(W13),"",NETWORKDAYS(TODAY(),W13,Conges!$B:$B))</f>
-        <v>19</v>
+      <c r="X13" s="19" t="str">
+        <f ca="1">IF(ISBLANK(W13),"",NETWORKDAYS(TODAY(),W13,Conges!$B:$B))</f>
+        <v/>
       </c>
     </row>
     <row r="14" spans="1:24">
       <c r="B14" s="13" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D14" s="5"/>
       <c r="G14" t="s">
+        <v>44</v>
+      </c>
+      <c r="L14" t="s">
         <v>45</v>
       </c>
-      <c r="L14" t="s">
+      <c r="Q14" t="s">
         <v>46</v>
-      </c>
-      <c r="Q14" t="s">
-        <v>47</v>
       </c>
       <c r="R14" s="5"/>
       <c r="W14" s="7"/>
       <c r="X14" s="19"/>
     </row>
     <row r="15" spans="1:24">
-      <c r="A15" t="s">
-        <f>IF(I62&lt;3,"X",IF(I62&lt;5,"x",""))</f>
-        <v>19</v>
-      </c>
-      <c r="B15" s="13" t="str">
-        <v>Finir modifs</v>
+      <c r="A15" t="str">
+        <f ca="1">IF(I62&lt;3,"X",IF(I62&lt;5,"x",""))</f>
+        <v/>
+      </c>
+      <c r="B15" s="13" t="s">
+        <v>111</v>
       </c>
       <c r="D15" s="5"/>
       <c r="G15" t="s">
+        <v>47</v>
+      </c>
+      <c r="L15" t="s">
         <v>48</v>
-      </c>
-      <c r="L15" t="s">
-        <v>49</v>
       </c>
       <c r="R15" s="5"/>
       <c r="W15" s="7"/>
     </row>
     <row r="16" spans="1:24">
-      <c r="A16" t="s">
-        <f>IF(I63&lt;3,"X",IF(I63&lt;5,"x",""))</f>
-        <v>19</v>
+      <c r="A16" t="str">
+        <f ca="1">IF(I63&lt;3,"X",IF(I63&lt;5,"x",""))</f>
+        <v/>
       </c>
       <c r="D16" s="5"/>
       <c r="L16" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="R16" s="5"/>
       <c r="V16" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="W16" s="7"/>
+    </row>
+    <row r="17" spans="1:24">
+      <c r="A17" t="str">
+        <f ca="1">IF(I64&lt;3,"X",IF(I64&lt;5,"x",""))</f>
+        <v/>
+      </c>
+      <c r="B17" s="8" t="s">
         <v>51</v>
-      </c>
-      <c r="W16" s="7"/>
-    </row>
-    <row r="17" spans="1:24">
-      <c r="A17" t="s">
-        <f>IF(I64&lt;3,"X",IF(I64&lt;5,"x",""))</f>
-        <v>19</v>
-      </c>
-      <c r="B17" s="8" t="s">
-        <v>52</v>
       </c>
       <c r="C17">
         <v>41911</v>
@@ -1383,30 +1595,30 @@
       <c r="H17" s="6"/>
       <c r="I17" s="22"/>
       <c r="L17" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q17" s="8" t="s">
         <v>53</v>
-      </c>
-      <c r="Q17" s="8" t="s">
-        <v>54</v>
       </c>
       <c r="R17" s="5"/>
       <c r="V17" t="s">
+        <v>54</v>
+      </c>
+      <c r="W17" s="7"/>
+    </row>
+    <row r="18" spans="1:24">
+      <c r="A18" t="str">
+        <f ca="1">IF(I65&lt;3,"X",IF(I65&lt;5,"x",""))</f>
+        <v/>
+      </c>
+      <c r="B18" s="23" t="s">
         <v>55</v>
-      </c>
-      <c r="W17" s="7"/>
-    </row>
-    <row r="18" spans="1:24">
-      <c r="A18" t="s">
-        <f>IF(I65&lt;3,"X",IF(I65&lt;5,"x",""))</f>
-        <v>19</v>
-      </c>
-      <c r="B18" s="23" t="s">
-        <v>56</v>
       </c>
       <c r="C18" s="5"/>
       <c r="D18" s="5"/>
       <c r="F18" s="4"/>
       <c r="G18" s="8" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="H18" s="6"/>
       <c r="I18" s="22"/>
@@ -1414,19 +1626,19 @@
       <c r="Q18" s="13"/>
       <c r="R18" s="5"/>
       <c r="V18" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="W18" s="7"/>
     </row>
     <row r="19" spans="1:24">
       <c r="B19" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C19" t="s">
         <v>5</v>
       </c>
       <c r="G19" s="23" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H19" s="6"/>
       <c r="I19" s="22"/>
@@ -1437,12 +1649,12 @@
       <c r="C20" s="5"/>
       <c r="D20" s="5"/>
       <c r="G20" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H20" s="6"/>
       <c r="I20" s="22"/>
       <c r="L20" s="8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="M20" s="6">
         <v>41695</v>
@@ -1457,19 +1669,19 @@
         <v>41988</v>
       </c>
       <c r="D21" s="25"/>
-      <c r="G21" s="13" t="str">
-        <v>Relance manu EDT</v>
+      <c r="G21" s="13" t="s">
+        <v>112</v>
       </c>
       <c r="H21" s="6"/>
       <c r="I21" s="22"/>
       <c r="L21" s="13" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="M21" s="6"/>
       <c r="P21" s="4"/>
       <c r="R21" s="5"/>
       <c r="V21" s="9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="W21" s="6">
         <v>41695</v>
@@ -1478,7 +1690,7 @@
     </row>
     <row r="22" spans="1:24">
       <c r="B22" s="8" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C22" s="5"/>
       <c r="D22" s="5"/>
@@ -1486,7 +1698,7 @@
       <c r="H22" s="6"/>
       <c r="I22" s="22"/>
       <c r="L22" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="M22" s="6"/>
       <c r="R22" s="5"/>
@@ -1504,7 +1716,7 @@
       <c r="I23" s="22"/>
       <c r="M23" s="6"/>
       <c r="Q23" s="8" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="R23" s="5"/>
     </row>
@@ -1513,51 +1725,51 @@
       <c r="C24" s="5"/>
       <c r="D24" s="5"/>
       <c r="G24" s="8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="H24" s="6"/>
       <c r="I24" s="22"/>
       <c r="M24" s="6"/>
       <c r="Q24" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="R24" s="5"/>
       <c r="V24" s="8" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="25" spans="1:24">
       <c r="A25" s="5"/>
       <c r="B25" s="8" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C25" s="5"/>
       <c r="D25" s="5"/>
       <c r="G25" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H25" s="6"/>
       <c r="I25" s="22"/>
-      <c r="L25" s="8" t="str">
-        <v>Task-Manager</v>
+      <c r="L25" s="8" t="s">
+        <v>113</v>
       </c>
       <c r="M25" s="6"/>
       <c r="Q25" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="R25" s="5"/>
     </row>
     <row r="26" spans="1:24">
       <c r="A26" s="5"/>
-      <c r="B26" s="13" t="str">
-        <v>Faire</v>
+      <c r="B26" s="13" t="s">
+        <v>114</v>
       </c>
       <c r="C26" s="5"/>
       <c r="D26" s="5"/>
       <c r="H26" s="6"/>
       <c r="I26" s="22"/>
-      <c r="L26" s="13" t="str">
-        <v>Spécification</v>
+      <c r="L26" s="13" t="s">
+        <v>115</v>
       </c>
       <c r="M26" s="6"/>
       <c r="Q26" s="13"/>
@@ -1565,13 +1777,13 @@
     </row>
     <row r="27" spans="1:24">
       <c r="A27" s="5"/>
-      <c r="B27" s="13" t="str">
-        <v>RdV</v>
+      <c r="B27" s="13" t="s">
+        <v>116</v>
       </c>
       <c r="C27" s="5"/>
       <c r="D27" s="5"/>
       <c r="G27" s="8" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="H27" s="6"/>
       <c r="I27" s="22"/>
@@ -1582,8 +1794,8 @@
       <c r="A28" s="5"/>
       <c r="C28" s="5"/>
       <c r="D28" s="5"/>
-      <c r="G28" s="13" t="str">
-        <v>Programme conf-call</v>
+      <c r="G28" s="13" t="s">
+        <v>117</v>
       </c>
       <c r="H28" s="6"/>
       <c r="I28" s="22"/>
@@ -1597,54 +1809,54 @@
     </row>
     <row r="30" spans="1:24">
       <c r="B30" s="28" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C30" s="28"/>
       <c r="D30" s="28"/>
       <c r="E30" s="28"/>
       <c r="F30" s="28"/>
       <c r="G30" s="28" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H30" s="28"/>
       <c r="I30" s="28"/>
       <c r="J30" s="28"/>
       <c r="K30" s="28"/>
       <c r="L30" s="28" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="M30" s="28"/>
       <c r="N30" s="28"/>
       <c r="O30" s="28"/>
       <c r="P30" s="28"/>
       <c r="Q30" s="28" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="31" spans="1:24">
       <c r="B31" s="29" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C31" s="29"/>
       <c r="D31" s="29"/>
       <c r="E31" s="29"/>
       <c r="F31" s="29"/>
       <c r="G31" s="29" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="H31" s="29"/>
       <c r="I31" s="29"/>
       <c r="J31" s="29"/>
       <c r="K31" s="29"/>
-      <c r="L31" s="29" t="str">
-        <v>Réponse DBLP</v>
+      <c r="L31" s="29" t="s">
+        <v>118</v>
       </c>
       <c r="M31" s="29"/>
       <c r="N31" s="29"/>
       <c r="O31" s="29"/>
       <c r="P31" s="29"/>
-      <c r="Q31" s="29" t="str">
-        <v>Manu: conflit EDT</v>
+      <c r="Q31" s="29" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="32" spans="1:24">
@@ -1670,28 +1882,28 @@
     </row>
     <row r="34" spans="1:24">
       <c r="B34" s="28" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C34" s="28"/>
       <c r="D34" s="28"/>
       <c r="E34" s="28"/>
       <c r="F34" s="28"/>
       <c r="G34" s="28" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="H34" s="28"/>
       <c r="I34" s="28"/>
       <c r="J34" s="28"/>
       <c r="K34" s="28"/>
       <c r="L34" s="28" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="M34" s="28"/>
       <c r="N34" s="28"/>
       <c r="O34" s="28"/>
       <c r="P34" s="28"/>
       <c r="Q34" s="28" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="35" spans="1:24">
@@ -1704,50 +1916,50 @@
     </row>
     <row r="37" spans="1:24">
       <c r="B37" s="28" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C37" s="28"/>
       <c r="D37" s="28"/>
       <c r="E37" s="28"/>
       <c r="F37" s="28"/>
       <c r="G37" s="28" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H37" s="28"/>
       <c r="I37" s="28"/>
       <c r="J37" s="28"/>
       <c r="K37" s="28"/>
       <c r="L37" s="28" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="M37" s="28"/>
       <c r="N37" s="28"/>
       <c r="O37" s="28"/>
       <c r="P37" s="28"/>
       <c r="Q37" s="28" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="39" spans="1:24">
       <c r="G39" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="L39" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="L39" s="8" t="s">
+      <c r="Q39" s="8" t="s">
         <v>81</v>
-      </c>
-      <c r="Q39" s="8" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="40" spans="1:24">
       <c r="B40" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="G40" t="s">
         <v>83</v>
       </c>
-      <c r="G40" t="s">
+      <c r="L40" t="s">
         <v>84</v>
-      </c>
-      <c r="L40" t="s">
-        <v>85</v>
       </c>
       <c r="Q40" s="13"/>
     </row>
@@ -1756,26 +1968,26 @@
     </row>
     <row r="42" spans="1:24">
       <c r="L42" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="Q42" s="8" t="s">
         <v>86</v>
-      </c>
-      <c r="Q42" s="8" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="43" spans="1:24">
       <c r="B43" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="L43" t="s">
         <v>88</v>
-      </c>
-      <c r="L43" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="44" spans="1:24">
       <c r="B44" t="s">
+        <v>89</v>
+      </c>
+      <c r="L44" t="s">
         <v>90</v>
-      </c>
-      <c r="L44" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="45" spans="1:24">
@@ -1783,36 +1995,36 @@
     </row>
     <row r="46" spans="1:24">
       <c r="G46" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="L46" s="8" t="s">
         <v>92</v>
-      </c>
-      <c r="L46" s="8" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="49" spans="1:24">
       <c r="B49" s="28" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C49" s="28"/>
       <c r="D49" s="28"/>
       <c r="E49" s="28"/>
       <c r="F49" s="28"/>
       <c r="G49" s="28" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H49" s="28"/>
       <c r="I49" s="28"/>
       <c r="J49" s="28"/>
       <c r="K49" s="28"/>
       <c r="L49" s="28" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="M49" s="28"/>
       <c r="N49" s="28"/>
       <c r="O49" s="28"/>
       <c r="P49" s="28"/>
       <c r="Q49" s="28" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="50" spans="1:24">
@@ -1822,15 +2034,15 @@
     </row>
     <row r="51" spans="1:24">
       <c r="B51" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C51" s="5"/>
       <c r="D51" s="5"/>
-      <c r="G51" t="str">
-        <v>Tel MAIF voiture</v>
-      </c>
-      <c r="L51" t="str">
-        <v>Tel karim Portet</v>
+      <c r="G51" t="s">
+        <v>120</v>
+      </c>
+      <c r="L51" t="s">
+        <v>121</v>
       </c>
       <c r="R51" s="5"/>
     </row>
@@ -1885,41 +2097,41 @@
     </row>
     <row r="61" spans="1:24">
       <c r="H61" s="6"/>
-      <c r="I61" s="30" t="s">
-        <f>IF(ISBLANK(H61),"",NETWORKDAYS(TODAY(),H61,Conges!$A:$A))</f>
-        <v>19</v>
+      <c r="I61" s="30" t="str">
+        <f ca="1">IF(ISBLANK(H61),"",NETWORKDAYS(TODAY(),H61,Conges!$A:$A))</f>
+        <v/>
       </c>
       <c r="M61" s="6"/>
     </row>
     <row r="62" spans="1:24">
       <c r="H62" s="6"/>
-      <c r="I62" s="31" t="s">
-        <f>IF(ISBLANK(H62),"",NETWORKDAYS(TODAY(),H62,Conges!$B:$B))</f>
-        <v>19</v>
+      <c r="I62" s="31" t="str">
+        <f ca="1">IF(ISBLANK(H62),"",NETWORKDAYS(TODAY(),H62,Conges!$B:$B))</f>
+        <v/>
       </c>
       <c r="M62" s="6"/>
     </row>
     <row r="63" spans="1:24">
       <c r="H63" s="6"/>
-      <c r="I63" s="31" t="s">
-        <f>IF(ISBLANK(H63),"",NETWORKDAYS(TODAY(),H63,Conges!$B:$B))</f>
-        <v>19</v>
+      <c r="I63" s="31" t="str">
+        <f ca="1">IF(ISBLANK(H63),"",NETWORKDAYS(TODAY(),H63,Conges!$B:$B))</f>
+        <v/>
       </c>
       <c r="M63" s="6"/>
     </row>
     <row r="64" spans="1:24">
       <c r="H64" s="6"/>
-      <c r="I64" s="31" t="s">
-        <f>IF(ISBLANK(H64),"",NETWORKDAYS(TODAY(),H64,Conges!$A:$A))</f>
-        <v>19</v>
+      <c r="I64" s="31" t="str">
+        <f ca="1">IF(ISBLANK(H64),"",NETWORKDAYS(TODAY(),H64,Conges!$A:$A))</f>
+        <v/>
       </c>
       <c r="M64" s="6"/>
     </row>
     <row r="65" spans="1:24">
       <c r="H65" s="6"/>
-      <c r="I65" s="31" t="s">
-        <f>IF(ISBLANK(H65),"",NETWORKDAYS(TODAY(),H65,Conges!$B:$B))</f>
-        <v>19</v>
+      <c r="I65" s="31" t="str">
+        <f ca="1">IF(ISBLANK(H65),"",NETWORKDAYS(TODAY(),H65,Conges!$B:$B))</f>
+        <v/>
       </c>
       <c r="M65" s="6"/>
     </row>
@@ -1948,46 +2160,42 @@
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" selectLockedCells="1" sort="0" autoFilter="0" pivotTables="0" selectUnlockedCells="1"/>
-  <printOptions/>
   <pageMargins left="1" right="1" top="1.667" bottom="1.667" header="1" footer="1"/>
-  <pageSetup blackAndWhite="0" cellComments="asDisplayed" draft="0" errors="displayed" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="0"/>
+  <pageSetup paperSize="9" orientation="portrait" cellComments="asDisplayed"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr>
-    <pageSetUpPr fitToPage="0"/>
-  </sheetPr>
-  <dimension ref="A1:X65536"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:IV65536"/>
   <sheetViews>
-    <sheetView workbookViewId="0" showOutlineSymbols="0">
+    <sheetView showOutlineSymbols="0" workbookViewId="0">
       <selection activeCell="B52" sqref="B52"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" style="34" width="2.856971" customWidth="1"/>
-    <col min="2" max="2" style="35" width="24.28425" customWidth="1"/>
-    <col min="3" max="3" style="36" width="5.285397" hidden="1" customWidth="1"/>
-    <col min="4" max="4" style="34" width="4.285457" customWidth="1"/>
-    <col min="5" max="5" style="35" width="4.285457" customWidth="1"/>
-    <col min="6" max="6" style="35" width="2.856971" customWidth="1"/>
-    <col min="7" max="7" style="35" width="24.28425" customWidth="1"/>
-    <col min="8" max="8" style="35" width="5.285397" hidden="1" customWidth="1"/>
-    <col min="9" max="10" style="35" width="4.285457" customWidth="1"/>
-    <col min="11" max="11" style="35" width="2.856971" customWidth="1"/>
-    <col min="12" max="12" style="35" width="24.28425" customWidth="1"/>
-    <col min="13" max="13" style="35" width="5.285397" hidden="1" customWidth="1"/>
-    <col min="14" max="15" style="35" width="4.285457" customWidth="1"/>
-    <col min="16" max="16" style="35" width="2.856971" customWidth="1"/>
-    <col min="17" max="17" style="35" width="24.28425" customWidth="1"/>
-    <col min="18" max="18" style="37" width="5.285397" hidden="1" customWidth="1"/>
-    <col min="19" max="20" style="35" width="4.285457" customWidth="1"/>
-    <col min="21" max="21" style="35" width="2.856971" customWidth="1"/>
-    <col min="22" max="22" style="35" width="24.28425" customWidth="1"/>
-    <col min="23" max="24" style="35" width="9.142308"/>
-    <col min="25" max="256" style="35"/>
+    <col min="1" max="1" width="2.875" style="34" customWidth="1"/>
+    <col min="2" max="2" width="24.25" style="35" customWidth="1"/>
+    <col min="3" max="3" width="5.25" style="36" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="4.25" style="34" customWidth="1"/>
+    <col min="5" max="5" width="4.25" style="35" customWidth="1"/>
+    <col min="6" max="6" width="2.875" style="35" customWidth="1"/>
+    <col min="7" max="7" width="24.25" style="35" customWidth="1"/>
+    <col min="8" max="8" width="5.25" style="35" hidden="1" customWidth="1"/>
+    <col min="9" max="10" width="4.25" style="35" customWidth="1"/>
+    <col min="11" max="11" width="2.875" style="35" customWidth="1"/>
+    <col min="12" max="12" width="24.25" style="35" customWidth="1"/>
+    <col min="13" max="13" width="5.25" style="35" hidden="1" customWidth="1"/>
+    <col min="14" max="15" width="4.25" style="35" customWidth="1"/>
+    <col min="16" max="16" width="2.875" style="35" customWidth="1"/>
+    <col min="17" max="17" width="24.25" style="35" customWidth="1"/>
+    <col min="18" max="18" width="5.25" style="37" hidden="1" customWidth="1"/>
+    <col min="19" max="20" width="4.25" style="35" customWidth="1"/>
+    <col min="21" max="21" width="2.875" style="35" customWidth="1"/>
+    <col min="22" max="22" width="24.25" style="35" customWidth="1"/>
+    <col min="23" max="24" width="9.125" style="35"/>
+    <col min="25" max="256" width="0" style="35" hidden="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:24">
@@ -2023,7 +2231,7 @@
     </row>
     <row r="2" spans="1:24">
       <c r="B2" s="39" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C2" t="s">
         <v>5</v>
@@ -2038,8 +2246,8 @@
         <v>41759</v>
       </c>
       <c r="I2" s="41">
-        <f>IF(ISBLANK(H2),"",NETWORKDAYS(TODAY(),H2,Conges!$B:$B))</f>
-        <v>192</v>
+        <f ca="1">IF(ISBLANK(H2),"",NETWORKDAYS(TODAY(),H2,Conges!$B:$B))</f>
+        <v>-208</v>
       </c>
       <c r="Q2" s="40" t="s">
         <v>11</v>
@@ -2073,57 +2281,57 @@
     </row>
     <row r="4" spans="1:24">
       <c r="B4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D4" s="42"/>
       <c r="G4" t="s">
         <v>18</v>
       </c>
       <c r="H4" s="36"/>
-      <c r="I4" s="41" t="s">
-        <f>IF(ISBLANK(H4),"",NETWORKDAYS(TODAY(),H4,Conges!$B:$B))</f>
-        <v>19</v>
+      <c r="I4" s="41" t="str">
+        <f ca="1">IF(ISBLANK(H4),"",NETWORKDAYS(TODAY(),H4,Conges!$B:$B))</f>
+        <v/>
       </c>
       <c r="L4" s="39"/>
       <c r="R4" s="35"/>
       <c r="V4" s="43" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="W4" s="37"/>
     </row>
     <row r="5" spans="1:24">
       <c r="B5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H5" s="36"/>
-      <c r="I5" s="41" t="s">
-        <f>IF(ISBLANK(H5),"",NETWORKDAYS(TODAY(),H5,Conges!$A:$A))</f>
-        <v>19</v>
+      <c r="I5" s="41" t="str">
+        <f ca="1">IF(ISBLANK(H5),"",NETWORKDAYS(TODAY(),H5,Conges!$A:$A))</f>
+        <v/>
       </c>
       <c r="L5" s="39"/>
       <c r="R5" s="35"/>
       <c r="V5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="W5" s="37"/>
     </row>
     <row r="6" spans="1:24">
-      <c r="B6" s="39" t="str">
-        <v>Imprimer doc MAJ Duco</v>
+      <c r="B6" s="39" t="s">
+        <v>122</v>
       </c>
       <c r="D6" s="44"/>
       <c r="G6" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q6" s="40" t="s">
         <v>25</v>
-      </c>
-      <c r="Q6" s="40" t="s">
-        <v>26</v>
       </c>
       <c r="R6" s="35"/>
       <c r="V6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="W6" s="37"/>
     </row>
@@ -2131,35 +2339,35 @@
       <c r="B7" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="45" t="s">
-        <f>IF(ISBLANK(C7),"",NETWORKDAYS(TODAY(),C7,Conges!$B:$B))</f>
-        <v>19</v>
+      <c r="D7" s="45" t="str">
+        <f ca="1">IF(ISBLANK(C7),"",NETWORKDAYS(TODAY(),C7,Conges!$B:$B))</f>
+        <v/>
       </c>
       <c r="G7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H7" s="36"/>
       <c r="L7" s="40" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q7" t="s">
         <v>29</v>
-      </c>
-      <c r="Q7" t="s">
-        <v>30</v>
       </c>
       <c r="R7" s="35"/>
       <c r="W7" s="37"/>
     </row>
     <row r="8" spans="1:24">
-      <c r="B8" t="str">
-        <v>Point Eric</v>
+      <c r="B8" t="s">
+        <v>123</v>
       </c>
       <c r="D8" s="35"/>
       <c r="H8" s="37"/>
       <c r="L8" s="39" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="R8" s="35"/>
       <c r="V8" s="40" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="W8" s="37"/>
     </row>
@@ -2173,11 +2381,11 @@
       <c r="I9" s="46"/>
       <c r="M9" s="37"/>
       <c r="Q9" s="40" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="R9" s="35"/>
       <c r="V9" s="47" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="W9" s="37"/>
     </row>
@@ -2187,11 +2395,11 @@
       <c r="L10" s="39"/>
       <c r="M10" s="36"/>
       <c r="Q10" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="R10" s="35"/>
       <c r="V10" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="W10" s="37"/>
     </row>
@@ -2199,16 +2407,16 @@
       <c r="A11" s="35"/>
       <c r="C11" s="35"/>
       <c r="D11" s="35"/>
-      <c r="F11" s="34" t="s">
+      <c r="F11" s="34" t="str">
         <f>IF(I12&lt;3,"X",IF(I12&lt;5,"x",""))</f>
-        <v>98</v>
+        <v>X</v>
       </c>
       <c r="Q11" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="R11" s="35"/>
       <c r="V11" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="W11" s="37"/>
     </row>
@@ -2218,107 +2426,107 @@
       <c r="D12" s="35"/>
       <c r="F12" s="34"/>
       <c r="G12" s="38" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H12" s="36"/>
       <c r="I12" s="48"/>
       <c r="L12" s="40" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q12" t="s">
         <v>36</v>
-      </c>
-      <c r="Q12" t="s">
-        <v>37</v>
       </c>
       <c r="R12" s="35"/>
       <c r="V12" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="W12" s="37">
         <v>41817</v>
       </c>
       <c r="X12" s="49">
-        <f>IF(ISBLANK(W12),"",NETWORKDAYS(TODAY(),W12,Conges!$B:$B))</f>
-        <v>150</v>
+        <f ca="1">IF(ISBLANK(W12),"",NETWORKDAYS(TODAY(),W12,Conges!$B:$B))</f>
+        <v>-166</v>
       </c>
     </row>
     <row r="13" spans="1:24">
       <c r="B13" s="38" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D13" s="35"/>
       <c r="G13" t="s">
+        <v>39</v>
+      </c>
+      <c r="L13" t="s">
         <v>40</v>
       </c>
-      <c r="L13" t="s">
+      <c r="Q13" s="50" t="s">
         <v>41</v>
-      </c>
-      <c r="Q13" s="50" t="s">
-        <v>42</v>
       </c>
       <c r="R13" s="35"/>
       <c r="V13" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="W13" s="37"/>
-      <c r="X13" s="49" t="s">
-        <f>IF(ISBLANK(W13),"",NETWORKDAYS(TODAY(),W13,Conges!$B:$B))</f>
-        <v>19</v>
+      <c r="X13" s="49" t="str">
+        <f ca="1">IF(ISBLANK(W13),"",NETWORKDAYS(TODAY(),W13,Conges!$B:$B))</f>
+        <v/>
       </c>
     </row>
     <row r="14" spans="1:24">
       <c r="B14" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D14" s="35"/>
       <c r="G14" t="s">
+        <v>44</v>
+      </c>
+      <c r="L14" t="s">
         <v>45</v>
       </c>
-      <c r="L14" t="s">
+      <c r="Q14" t="s">
         <v>46</v>
-      </c>
-      <c r="Q14" t="s">
-        <v>47</v>
       </c>
       <c r="R14" s="35"/>
       <c r="W14" s="37"/>
       <c r="X14" s="49"/>
     </row>
     <row r="15" spans="1:24">
-      <c r="A15" t="s">
-        <f>IF(I62&lt;3,"X",IF(I62&lt;5,"x",""))</f>
-        <v>19</v>
+      <c r="A15" t="str">
+        <f ca="1">IF(I62&lt;3,"X",IF(I62&lt;5,"x",""))</f>
+        <v/>
       </c>
       <c r="D15" s="35"/>
       <c r="G15" t="s">
+        <v>47</v>
+      </c>
+      <c r="L15" t="s">
         <v>48</v>
-      </c>
-      <c r="L15" t="s">
-        <v>49</v>
       </c>
       <c r="R15" s="35"/>
       <c r="W15" s="37"/>
     </row>
     <row r="16" spans="1:24">
-      <c r="A16" t="s">
-        <f>IF(I63&lt;3,"X",IF(I63&lt;5,"x",""))</f>
-        <v>19</v>
+      <c r="A16" t="str">
+        <f ca="1">IF(I63&lt;3,"X",IF(I63&lt;5,"x",""))</f>
+        <v/>
       </c>
       <c r="D16" s="35"/>
       <c r="L16" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="R16" s="35"/>
       <c r="V16" s="40" t="s">
+        <v>50</v>
+      </c>
+      <c r="W16" s="37"/>
+    </row>
+    <row r="17" spans="1:24">
+      <c r="A17" t="str">
+        <f ca="1">IF(I64&lt;3,"X",IF(I64&lt;5,"x",""))</f>
+        <v/>
+      </c>
+      <c r="B17" s="38" t="s">
         <v>51</v>
-      </c>
-      <c r="W16" s="37"/>
-    </row>
-    <row r="17" spans="1:24">
-      <c r="A17" t="s">
-        <f>IF(I64&lt;3,"X",IF(I64&lt;5,"x",""))</f>
-        <v>19</v>
-      </c>
-      <c r="B17" s="38" t="s">
-        <v>52</v>
       </c>
       <c r="C17">
         <v>41911</v>
@@ -2327,52 +2535,52 @@
       <c r="H17" s="36"/>
       <c r="I17" s="52"/>
       <c r="L17" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q17" s="38" t="s">
         <v>53</v>
-      </c>
-      <c r="Q17" s="38" t="s">
-        <v>54</v>
       </c>
       <c r="R17" s="35"/>
       <c r="V17" t="s">
+        <v>54</v>
+      </c>
+      <c r="W17" s="37"/>
+    </row>
+    <row r="18" spans="1:24">
+      <c r="A18" t="str">
+        <f ca="1">IF(I65&lt;3,"X",IF(I65&lt;5,"x",""))</f>
+        <v/>
+      </c>
+      <c r="B18" s="53" t="s">
         <v>55</v>
-      </c>
-      <c r="W17" s="37"/>
-    </row>
-    <row r="18" spans="1:24">
-      <c r="A18" t="s">
-        <f>IF(I65&lt;3,"X",IF(I65&lt;5,"x",""))</f>
-        <v>19</v>
-      </c>
-      <c r="B18" s="53" t="s">
-        <v>56</v>
       </c>
       <c r="C18" s="35"/>
       <c r="D18" s="35"/>
       <c r="F18" s="34"/>
       <c r="G18" s="38" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="H18" s="36"/>
       <c r="I18" s="52"/>
       <c r="L18" s="39"/>
-      <c r="Q18" s="39" t="str">
-        <v>Organiser réunion Airbus</v>
+      <c r="Q18" s="39" t="s">
+        <v>124</v>
       </c>
       <c r="R18" s="35"/>
       <c r="V18" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="W18" s="37"/>
     </row>
     <row r="19" spans="1:24">
       <c r="B19" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C19" t="s">
         <v>5</v>
       </c>
       <c r="G19" s="53" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H19" s="36"/>
       <c r="I19" s="52"/>
@@ -2383,12 +2591,12 @@
       <c r="C20" s="35"/>
       <c r="D20" s="35"/>
       <c r="G20" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H20" s="36"/>
       <c r="I20" s="52"/>
       <c r="L20" s="38" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="M20" s="36">
         <v>41695</v>
@@ -2410,7 +2618,7 @@
       <c r="P21" s="34"/>
       <c r="R21" s="35"/>
       <c r="V21" s="40" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="W21" s="36">
         <v>41695</v>
@@ -2419,7 +2627,7 @@
     </row>
     <row r="22" spans="1:24">
       <c r="B22" s="38" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C22" s="35"/>
       <c r="D22" s="35"/>
@@ -2443,7 +2651,7 @@
       <c r="I23" s="52"/>
       <c r="M23" s="36"/>
       <c r="Q23" s="38" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="R23" s="35"/>
     </row>
@@ -2452,40 +2660,40 @@
       <c r="C24" s="35"/>
       <c r="D24" s="35"/>
       <c r="G24" s="38" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="H24" s="36"/>
       <c r="I24" s="52"/>
       <c r="L24" s="38" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="M24" s="36"/>
       <c r="Q24" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="R24" s="35"/>
       <c r="V24" s="38" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="25" spans="1:24">
       <c r="A25" s="35"/>
       <c r="B25" s="38" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C25" s="35"/>
       <c r="D25" s="35"/>
       <c r="G25" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H25" s="36"/>
       <c r="I25" s="52"/>
       <c r="L25" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="M25" s="36"/>
       <c r="Q25" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="R25" s="35"/>
     </row>
@@ -2496,11 +2704,11 @@
       <c r="H26" s="36"/>
       <c r="I26" s="52"/>
       <c r="L26" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="M26" s="36"/>
-      <c r="Q26" s="39" t="str">
-        <v>Fred: co-tutelle Barcelone</v>
+      <c r="Q26" s="39" t="s">
+        <v>125</v>
       </c>
       <c r="R26" s="35"/>
     </row>
@@ -2509,7 +2717,7 @@
       <c r="C27" s="35"/>
       <c r="D27" s="35"/>
       <c r="G27" s="38" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="H27" s="36"/>
       <c r="I27" s="52"/>
@@ -2520,8 +2728,8 @@
       <c r="A28" s="35"/>
       <c r="C28" s="35"/>
       <c r="D28" s="35"/>
-      <c r="G28" s="39" t="str">
-        <v>Répondre Barberis</v>
+      <c r="G28" s="39" t="s">
+        <v>126</v>
       </c>
       <c r="H28" s="36"/>
       <c r="I28" s="52"/>
@@ -2535,40 +2743,40 @@
     </row>
     <row r="30" spans="1:24">
       <c r="B30" s="58" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C30" s="58"/>
       <c r="D30" s="58"/>
       <c r="E30" s="58"/>
       <c r="F30" s="58"/>
       <c r="G30" s="58" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H30" s="58"/>
       <c r="I30" s="58"/>
       <c r="J30" s="58"/>
       <c r="K30" s="58"/>
       <c r="L30" s="58" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="M30" s="58"/>
       <c r="N30" s="58"/>
       <c r="O30" s="58"/>
       <c r="P30" s="58"/>
       <c r="Q30" s="58" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="31" spans="1:24">
       <c r="B31" s="59" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C31" s="59"/>
       <c r="D31" s="59"/>
       <c r="E31" s="59"/>
       <c r="F31" s="59"/>
       <c r="G31" s="59" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="H31" s="59"/>
       <c r="I31" s="59"/>
@@ -2604,28 +2812,28 @@
     </row>
     <row r="34" spans="1:24">
       <c r="B34" s="58" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C34" s="58"/>
       <c r="D34" s="58"/>
       <c r="E34" s="58"/>
       <c r="F34" s="58"/>
       <c r="G34" s="58" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="H34" s="58"/>
       <c r="I34" s="58"/>
       <c r="J34" s="58"/>
       <c r="K34" s="58"/>
       <c r="L34" s="58" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="M34" s="58"/>
       <c r="N34" s="58"/>
       <c r="O34" s="58"/>
       <c r="P34" s="58"/>
       <c r="Q34" s="58" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="35" spans="1:24">
@@ -2638,127 +2846,127 @@
     </row>
     <row r="37" spans="1:24">
       <c r="B37" s="58" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C37" s="58"/>
       <c r="D37" s="58"/>
       <c r="E37" s="58"/>
       <c r="F37" s="58"/>
       <c r="G37" s="58" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H37" s="58"/>
       <c r="I37" s="58"/>
       <c r="J37" s="58"/>
       <c r="K37" s="58"/>
       <c r="L37" s="58" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="M37" s="58"/>
       <c r="N37" s="58"/>
       <c r="O37" s="58"/>
       <c r="P37" s="58"/>
       <c r="Q37" s="58" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="39" spans="1:24">
       <c r="G39" s="38" t="s">
+        <v>79</v>
+      </c>
+      <c r="L39" s="38" t="s">
         <v>80</v>
       </c>
-      <c r="L39" s="38" t="s">
+      <c r="Q39" s="38" t="s">
         <v>81</v>
-      </c>
-      <c r="Q39" s="38" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="40" spans="1:24">
       <c r="B40" s="38" t="s">
+        <v>82</v>
+      </c>
+      <c r="G40" t="s">
         <v>83</v>
       </c>
-      <c r="G40" t="s">
+      <c r="L40" t="s">
         <v>84</v>
       </c>
-      <c r="L40" t="s">
-        <v>85</v>
-      </c>
       <c r="Q40" s="39" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="41" spans="1:24">
       <c r="Q41" s="39" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="42" spans="1:24">
       <c r="L42" s="38" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="43" spans="1:24">
       <c r="B43" s="38" t="s">
+        <v>87</v>
+      </c>
+      <c r="L43" t="s">
         <v>88</v>
-      </c>
-      <c r="L43" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="44" spans="1:24">
       <c r="B44" t="s">
+        <v>89</v>
+      </c>
+      <c r="L44" t="s">
         <v>90</v>
-      </c>
-      <c r="L44" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="45" spans="1:24">
       <c r="B45" s="39"/>
       <c r="Q45" s="38" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="46" spans="1:24">
       <c r="G46" s="38" t="s">
+        <v>91</v>
+      </c>
+      <c r="L46" s="38" t="s">
         <v>92</v>
       </c>
-      <c r="L46" s="38" t="s">
-        <v>93</v>
-      </c>
       <c r="Q46" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="47" spans="1:24">
       <c r="Q47" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="49" spans="1:24">
       <c r="B49" s="58" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C49" s="58"/>
       <c r="D49" s="58"/>
       <c r="E49" s="58"/>
       <c r="F49" s="58"/>
       <c r="G49" s="58" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H49" s="58"/>
       <c r="I49" s="58"/>
       <c r="J49" s="58"/>
       <c r="K49" s="58"/>
       <c r="L49" s="58" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="M49" s="58"/>
       <c r="N49" s="58"/>
       <c r="O49" s="58"/>
       <c r="P49" s="58"/>
       <c r="Q49" s="58" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="50" spans="1:24">
@@ -2768,7 +2976,7 @@
     </row>
     <row r="51" spans="1:24">
       <c r="B51" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C51" s="35"/>
       <c r="D51" s="35"/>
@@ -2827,41 +3035,41 @@
     </row>
     <row r="61" spans="1:24">
       <c r="H61" s="36"/>
-      <c r="I61" s="60" t="s">
-        <f>IF(ISBLANK(H61),"",NETWORKDAYS(TODAY(),H61,Conges!$A:$A))</f>
-        <v>19</v>
+      <c r="I61" s="60" t="str">
+        <f ca="1">IF(ISBLANK(H61),"",NETWORKDAYS(TODAY(),H61,Conges!$A:$A))</f>
+        <v/>
       </c>
       <c r="M61" s="36"/>
     </row>
     <row r="62" spans="1:24">
       <c r="H62" s="36"/>
-      <c r="I62" s="61" t="s">
-        <f>IF(ISBLANK(H62),"",NETWORKDAYS(TODAY(),H62,Conges!$B:$B))</f>
-        <v>19</v>
+      <c r="I62" s="61" t="str">
+        <f ca="1">IF(ISBLANK(H62),"",NETWORKDAYS(TODAY(),H62,Conges!$B:$B))</f>
+        <v/>
       </c>
       <c r="M62" s="36"/>
     </row>
     <row r="63" spans="1:24">
       <c r="H63" s="36"/>
-      <c r="I63" s="61" t="s">
-        <f>IF(ISBLANK(H63),"",NETWORKDAYS(TODAY(),H63,Conges!$B:$B))</f>
-        <v>19</v>
+      <c r="I63" s="61" t="str">
+        <f ca="1">IF(ISBLANK(H63),"",NETWORKDAYS(TODAY(),H63,Conges!$B:$B))</f>
+        <v/>
       </c>
       <c r="M63" s="36"/>
     </row>
     <row r="64" spans="1:24">
       <c r="H64" s="36"/>
-      <c r="I64" s="61" t="s">
-        <f>IF(ISBLANK(H64),"",NETWORKDAYS(TODAY(),H64,Conges!$A:$A))</f>
-        <v>19</v>
+      <c r="I64" s="61" t="str">
+        <f ca="1">IF(ISBLANK(H64),"",NETWORKDAYS(TODAY(),H64,Conges!$A:$A))</f>
+        <v/>
       </c>
       <c r="M64" s="36"/>
     </row>
     <row r="65" spans="1:24">
       <c r="H65" s="36"/>
-      <c r="I65" s="61" t="s">
-        <f>IF(ISBLANK(H65),"",NETWORKDAYS(TODAY(),H65,Conges!$B:$B))</f>
-        <v>19</v>
+      <c r="I65" s="61" t="str">
+        <f ca="1">IF(ISBLANK(H65),"",NETWORKDAYS(TODAY(),H65,Conges!$B:$B))</f>
+        <v/>
       </c>
       <c r="M65" s="36"/>
     </row>
@@ -2890,51 +3098,47 @@
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" selectLockedCells="1" sort="0" autoFilter="0" pivotTables="0" selectUnlockedCells="1"/>
-  <printOptions/>
   <pageMargins left="1" right="1" top="1.667" bottom="1.667" header="1" footer="1"/>
-  <pageSetup blackAndWhite="0" cellComments="asDisplayed" draft="0" errors="displayed" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="0"/>
+  <pageSetup paperSize="9" orientation="portrait" cellComments="asDisplayed"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr>
-    <pageSetUpPr fitToPage="0"/>
-  </sheetPr>
-  <dimension ref="A1:X65536"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:IV65536"/>
   <sheetViews>
-    <sheetView workbookViewId="0" showOutlineSymbols="0">
+    <sheetView showOutlineSymbols="0" workbookViewId="0">
       <selection activeCell="B50" sqref="B50"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" style="64" width="2.856971" customWidth="1"/>
-    <col min="2" max="2" style="65" width="24.28425" customWidth="1"/>
-    <col min="3" max="3" style="66" width="5.285397" hidden="1" customWidth="1"/>
-    <col min="4" max="4" style="64" width="4.285457" customWidth="1"/>
-    <col min="5" max="5" style="65" width="4.285457" customWidth="1"/>
-    <col min="6" max="6" style="65" width="2.856971" customWidth="1"/>
-    <col min="7" max="7" style="65" width="24.28425" customWidth="1"/>
-    <col min="8" max="8" style="65" width="5.285397" hidden="1" customWidth="1"/>
-    <col min="9" max="10" style="65" width="4.285457" customWidth="1"/>
-    <col min="11" max="11" style="65" width="2.856971" customWidth="1"/>
-    <col min="12" max="12" style="65" width="24.28425" customWidth="1"/>
-    <col min="13" max="13" style="65" width="5.285397" hidden="1" customWidth="1"/>
-    <col min="14" max="15" style="65" width="4.285457" customWidth="1"/>
-    <col min="16" max="16" style="65" width="2.856971" customWidth="1"/>
-    <col min="17" max="17" style="65" width="24.28425" customWidth="1"/>
-    <col min="18" max="18" style="67" width="5.285397" hidden="1" customWidth="1"/>
-    <col min="19" max="20" style="65" width="4.285457" customWidth="1"/>
-    <col min="21" max="21" style="65" width="2.856971" customWidth="1"/>
-    <col min="22" max="22" style="65" width="24.28425" customWidth="1"/>
-    <col min="23" max="24" style="65" width="9.142308"/>
-    <col min="25" max="256" style="65"/>
+    <col min="1" max="1" width="2.875" style="64" customWidth="1"/>
+    <col min="2" max="2" width="24.25" style="65" customWidth="1"/>
+    <col min="3" max="3" width="5.25" style="66" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="4.25" style="64" customWidth="1"/>
+    <col min="5" max="5" width="4.25" style="65" customWidth="1"/>
+    <col min="6" max="6" width="2.875" style="65" customWidth="1"/>
+    <col min="7" max="7" width="24.25" style="65" customWidth="1"/>
+    <col min="8" max="8" width="5.25" style="65" hidden="1" customWidth="1"/>
+    <col min="9" max="10" width="4.25" style="65" customWidth="1"/>
+    <col min="11" max="11" width="2.875" style="65" customWidth="1"/>
+    <col min="12" max="12" width="24.25" style="65" customWidth="1"/>
+    <col min="13" max="13" width="5.25" style="65" hidden="1" customWidth="1"/>
+    <col min="14" max="15" width="4.25" style="65" customWidth="1"/>
+    <col min="16" max="16" width="2.875" style="65" customWidth="1"/>
+    <col min="17" max="17" width="24.25" style="65" customWidth="1"/>
+    <col min="18" max="18" width="5.25" style="67" hidden="1" customWidth="1"/>
+    <col min="19" max="20" width="4.25" style="65" customWidth="1"/>
+    <col min="21" max="21" width="2.875" style="65" customWidth="1"/>
+    <col min="22" max="22" width="24.25" style="65" customWidth="1"/>
+    <col min="23" max="24" width="9.125" style="65"/>
+    <col min="25" max="256" width="0" style="65" hidden="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:24">
-      <c r="B1" s="68" t="str">
-        <v>HP15</v>
+      <c r="B1" s="68" t="s">
+        <v>127</v>
       </c>
       <c r="D1" t="s">
         <v>2</v>
@@ -2964,8 +3168,8 @@
       </c>
     </row>
     <row r="2" spans="1:24">
-      <c r="B2" s="70" t="str">
-        <v>Bilan</v>
+      <c r="B2" s="70" t="s">
+        <v>128</v>
       </c>
       <c r="C2" t="s">
         <v>5</v>
@@ -2980,11 +3184,11 @@
         <v>41759</v>
       </c>
       <c r="I2" s="72">
-        <f>IF(ISBLANK(H2),"",NETWORKDAYS(TODAY(),H2,Conges!$B:$B))</f>
-        <v>192</v>
+        <f ca="1">IF(ISBLANK(H2),"",NETWORKDAYS(TODAY(),H2,Conges!$B:$B))</f>
+        <v>-208</v>
       </c>
       <c r="L2" s="71" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="Q2" s="71" t="s">
         <v>11</v>
@@ -3005,8 +3209,8 @@
         <v>41697</v>
       </c>
       <c r="I3" s="72"/>
-      <c r="L3" t="str">
-        <v>Transfert</v>
+      <c r="L3" t="s">
+        <v>129</v>
       </c>
       <c r="Q3" t="s">
         <v>15</v>
@@ -3026,33 +3230,33 @@
         <v>18</v>
       </c>
       <c r="H4" s="66"/>
-      <c r="I4" s="72" t="s">
-        <f>IF(ISBLANK(H4),"",NETWORKDAYS(TODAY(),H4,Conges!$B:$B))</f>
-        <v>19</v>
+      <c r="I4" s="72" t="str">
+        <f ca="1">IF(ISBLANK(H4),"",NETWORKDAYS(TODAY(),H4,Conges!$B:$B))</f>
+        <v/>
       </c>
       <c r="L4" s="70"/>
       <c r="R4" s="65"/>
       <c r="V4" s="75" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="W4" s="67"/>
     </row>
     <row r="5" spans="1:24">
       <c r="B5" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H5" s="66"/>
-      <c r="I5" s="72" t="s">
-        <f>IF(ISBLANK(H5),"",NETWORKDAYS(TODAY(),H5,Conges!$A:$A))</f>
-        <v>19</v>
+      <c r="I5" s="72" t="str">
+        <f ca="1">IF(ISBLANK(H5),"",NETWORKDAYS(TODAY(),H5,Conges!$A:$A))</f>
+        <v/>
       </c>
       <c r="L5" s="70"/>
       <c r="R5" s="65"/>
       <c r="V5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="W5" s="67"/>
     </row>
@@ -3062,50 +3266,50 @@
       </c>
       <c r="D6" s="76"/>
       <c r="G6" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q6" s="71" t="s">
         <v>25</v>
-      </c>
-      <c r="Q6" s="71" t="s">
-        <v>26</v>
       </c>
       <c r="R6" s="65"/>
       <c r="V6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="W6" s="67"/>
     </row>
     <row r="7" spans="1:24">
       <c r="B7" t="s">
-        <v>21</v>
-      </c>
-      <c r="D7" s="77" t="s">
-        <f>IF(ISBLANK(C7),"",NETWORKDAYS(TODAY(),C7,Conges!$B:$B))</f>
-        <v>19</v>
+        <v>20</v>
+      </c>
+      <c r="D7" s="77" t="str">
+        <f ca="1">IF(ISBLANK(C7),"",NETWORKDAYS(TODAY(),C7,Conges!$B:$B))</f>
+        <v/>
       </c>
       <c r="G7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H7" s="66"/>
       <c r="L7" s="71" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q7" t="s">
         <v>29</v>
-      </c>
-      <c r="Q7" t="s">
-        <v>30</v>
       </c>
       <c r="R7" s="65"/>
       <c r="W7" s="67"/>
     </row>
     <row r="8" spans="1:24">
       <c r="B8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D8" s="65"/>
       <c r="H8" s="67"/>
       <c r="L8" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="R8" s="65"/>
       <c r="V8" s="71" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="W8" s="67"/>
     </row>
@@ -3116,11 +3320,11 @@
       <c r="I9" s="78"/>
       <c r="M9" s="67"/>
       <c r="Q9" s="71" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="R9" s="65"/>
       <c r="V9" s="79" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="W9" s="67"/>
     </row>
@@ -3130,11 +3334,11 @@
       <c r="L10" s="70"/>
       <c r="M10" s="66"/>
       <c r="Q10" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="R10" s="65"/>
       <c r="V10" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="W10" s="67"/>
     </row>
@@ -3142,16 +3346,16 @@
       <c r="A11" s="65"/>
       <c r="C11" s="65"/>
       <c r="D11" s="65"/>
-      <c r="F11" s="64" t="s">
+      <c r="F11" s="64" t="str">
         <f>IF(I12&lt;3,"X",IF(I12&lt;5,"x",""))</f>
-        <v>98</v>
+        <v>X</v>
       </c>
       <c r="Q11" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="R11" s="65"/>
       <c r="V11" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="W11" s="67"/>
     </row>
@@ -3161,107 +3365,107 @@
       <c r="D12" s="65"/>
       <c r="F12" s="64"/>
       <c r="G12" s="69" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H12" s="66"/>
       <c r="I12" s="80"/>
       <c r="L12" s="71" t="s">
-        <v>36</v>
-      </c>
-      <c r="Q12" t="str">
-        <v>Surveiller svn</v>
+        <v>35</v>
+      </c>
+      <c r="Q12" t="s">
+        <v>130</v>
       </c>
       <c r="R12" s="65"/>
       <c r="V12" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="W12" s="67">
         <v>41817</v>
       </c>
       <c r="X12" s="81">
-        <f>IF(ISBLANK(W12),"",NETWORKDAYS(TODAY(),W12,Conges!$B:$B))</f>
-        <v>150</v>
+        <f ca="1">IF(ISBLANK(W12),"",NETWORKDAYS(TODAY(),W12,Conges!$B:$B))</f>
+        <v>-166</v>
       </c>
     </row>
     <row r="13" spans="1:24">
       <c r="B13" s="69" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D13" s="65"/>
       <c r="G13" t="s">
+        <v>39</v>
+      </c>
+      <c r="L13" t="s">
         <v>40</v>
       </c>
-      <c r="L13" t="s">
+      <c r="Q13" s="82" t="s">
         <v>41</v>
-      </c>
-      <c r="Q13" s="82" t="s">
-        <v>42</v>
       </c>
       <c r="R13" s="65"/>
       <c r="V13" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="W13" s="67"/>
-      <c r="X13" s="81" t="s">
-        <f>IF(ISBLANK(W13),"",NETWORKDAYS(TODAY(),W13,Conges!$B:$B))</f>
-        <v>19</v>
+      <c r="X13" s="81" t="str">
+        <f ca="1">IF(ISBLANK(W13),"",NETWORKDAYS(TODAY(),W13,Conges!$B:$B))</f>
+        <v/>
       </c>
     </row>
     <row r="14" spans="1:24">
       <c r="B14" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D14" s="65"/>
       <c r="G14" t="s">
+        <v>44</v>
+      </c>
+      <c r="L14" t="s">
         <v>45</v>
-      </c>
-      <c r="L14" t="s">
-        <v>46</v>
       </c>
       <c r="R14" s="65"/>
       <c r="W14" s="67"/>
       <c r="X14" s="81"/>
     </row>
     <row r="15" spans="1:24">
-      <c r="A15" t="s">
-        <f>IF(I60&lt;3,"X",IF(I60&lt;5,"x",""))</f>
-        <v>19</v>
-      </c>
-      <c r="B15" s="70" t="str">
-        <v>Relire</v>
+      <c r="A15" t="str">
+        <f ca="1">IF(I60&lt;3,"X",IF(I60&lt;5,"x",""))</f>
+        <v/>
+      </c>
+      <c r="B15" s="70" t="s">
+        <v>131</v>
       </c>
       <c r="D15" s="65"/>
       <c r="G15" t="s">
+        <v>47</v>
+      </c>
+      <c r="L15" t="s">
         <v>48</v>
-      </c>
-      <c r="L15" t="s">
-        <v>49</v>
       </c>
       <c r="R15" s="65"/>
       <c r="W15" s="67"/>
     </row>
     <row r="16" spans="1:24">
-      <c r="A16" t="s">
-        <f>IF(I61&lt;3,"X",IF(I61&lt;5,"x",""))</f>
-        <v>19</v>
+      <c r="A16" t="str">
+        <f ca="1">IF(I61&lt;3,"X",IF(I61&lt;5,"x",""))</f>
+        <v/>
       </c>
       <c r="D16" s="65"/>
       <c r="L16" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="R16" s="65"/>
       <c r="V16" s="71" t="s">
+        <v>50</v>
+      </c>
+      <c r="W16" s="67"/>
+    </row>
+    <row r="17" spans="1:24">
+      <c r="A17" t="str">
+        <f ca="1">IF(I62&lt;3,"X",IF(I62&lt;5,"x",""))</f>
+        <v/>
+      </c>
+      <c r="B17" s="69" t="s">
         <v>51</v>
-      </c>
-      <c r="W16" s="67"/>
-    </row>
-    <row r="17" spans="1:24">
-      <c r="A17" t="s">
-        <f>IF(I62&lt;3,"X",IF(I62&lt;5,"x",""))</f>
-        <v>19</v>
-      </c>
-      <c r="B17" s="69" t="s">
-        <v>52</v>
       </c>
       <c r="C17">
         <v>41911</v>
@@ -3270,37 +3474,37 @@
       <c r="H17" s="66"/>
       <c r="I17" s="84"/>
       <c r="L17" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q17" s="69" t="s">
         <v>53</v>
-      </c>
-      <c r="Q17" s="69" t="s">
-        <v>54</v>
       </c>
       <c r="R17" s="65"/>
       <c r="V17" t="s">
+        <v>54</v>
+      </c>
+      <c r="W17" s="67"/>
+    </row>
+    <row r="18" spans="1:24">
+      <c r="A18" t="str">
+        <f ca="1">IF(I63&lt;3,"X",IF(I63&lt;5,"x",""))</f>
+        <v/>
+      </c>
+      <c r="B18" t="s">
         <v>55</v>
-      </c>
-      <c r="W17" s="67"/>
-    </row>
-    <row r="18" spans="1:24">
-      <c r="A18" t="s">
-        <f>IF(I63&lt;3,"X",IF(I63&lt;5,"x",""))</f>
-        <v>19</v>
-      </c>
-      <c r="B18" t="s">
-        <v>56</v>
       </c>
       <c r="C18" s="65"/>
       <c r="D18" s="65"/>
       <c r="F18" s="64"/>
       <c r="G18" s="69" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="H18" s="66"/>
       <c r="I18" s="84"/>
       <c r="L18" s="70"/>
       <c r="R18" s="65"/>
       <c r="V18" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="W18" s="67"/>
     </row>
@@ -3308,8 +3512,8 @@
       <c r="C19" t="s">
         <v>5</v>
       </c>
-      <c r="G19" s="70" t="str">
-        <v>Voir EDT</v>
+      <c r="G19" s="70" t="s">
+        <v>132</v>
       </c>
       <c r="H19" s="66"/>
       <c r="I19" s="84"/>
@@ -3319,13 +3523,13 @@
     <row r="20" spans="1:24">
       <c r="C20" s="65"/>
       <c r="D20" s="65"/>
-      <c r="G20" s="70" t="str">
-        <v>Répondre sécu Carlos</v>
+      <c r="G20" s="70" t="s">
+        <v>133</v>
       </c>
       <c r="H20" s="66"/>
       <c r="I20" s="84"/>
       <c r="L20" s="69" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="M20" s="66">
         <v>41695</v>
@@ -3341,18 +3545,18 @@
       </c>
       <c r="D21" s="86"/>
       <c r="G21" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H21" s="66"/>
       <c r="I21" s="84"/>
-      <c r="L21" s="70" t="str">
-        <v>relance Eric/Lachaize/Xentium/Recore</v>
+      <c r="L21" s="70" t="s">
+        <v>134</v>
       </c>
       <c r="M21" s="66"/>
       <c r="P21" s="64"/>
       <c r="R21" s="65"/>
       <c r="V21" s="71" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="W21" s="66">
         <v>41695</v>
@@ -3361,17 +3565,17 @@
     </row>
     <row r="22" spans="1:24">
       <c r="B22" s="69" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C22" s="65"/>
       <c r="D22" s="65"/>
-      <c r="G22" s="70" t="str">
-        <v>Répondre Lyne</v>
+      <c r="G22" s="70" t="s">
+        <v>135</v>
       </c>
       <c r="H22" s="66"/>
       <c r="I22" s="84"/>
-      <c r="L22" s="70" t="str">
-        <v>mail Kalray</v>
+      <c r="L22" s="70" t="s">
+        <v>136</v>
       </c>
       <c r="M22" s="66"/>
       <c r="R22" s="65"/>
@@ -3389,7 +3593,7 @@
       <c r="I23" s="84"/>
       <c r="M23" s="66"/>
       <c r="Q23" s="69" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="R23" s="65"/>
     </row>
@@ -3398,40 +3602,40 @@
       <c r="C24" s="65"/>
       <c r="D24" s="65"/>
       <c r="G24" s="69" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="H24" s="66"/>
       <c r="I24" s="84"/>
       <c r="L24" s="69" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="M24" s="66"/>
       <c r="Q24" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="R24" s="65"/>
       <c r="V24" s="69" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="25" spans="1:24">
       <c r="A25" s="65"/>
       <c r="B25" s="69" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C25" s="65"/>
       <c r="D25" s="65"/>
       <c r="G25" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H25" s="66"/>
       <c r="I25" s="84"/>
-      <c r="L25" s="70" t="str">
-        <v>EasyChair</v>
+      <c r="L25" s="70" t="s">
+        <v>137</v>
       </c>
       <c r="M25" s="66"/>
       <c r="Q25" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="R25" s="65"/>
     </row>
@@ -3469,28 +3673,28 @@
     </row>
     <row r="30" spans="1:24">
       <c r="B30" s="89" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C30" s="89"/>
       <c r="D30" s="89"/>
       <c r="E30" s="89"/>
       <c r="F30" s="89"/>
       <c r="G30" s="89" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="H30" s="89"/>
       <c r="I30" s="89"/>
       <c r="J30" s="89"/>
       <c r="K30" s="89"/>
       <c r="L30" s="89" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="M30" s="89"/>
       <c r="N30" s="89"/>
       <c r="O30" s="89"/>
       <c r="P30" s="89"/>
       <c r="Q30" s="89" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="31" spans="1:24">
@@ -3511,133 +3715,133 @@
     </row>
     <row r="35" spans="1:24">
       <c r="B35" s="89" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C35" s="89"/>
       <c r="D35" s="89"/>
       <c r="E35" s="89"/>
       <c r="F35" s="89"/>
       <c r="G35" s="89" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H35" s="89"/>
       <c r="I35" s="89"/>
       <c r="J35" s="89"/>
       <c r="K35" s="89"/>
       <c r="L35" s="89" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="M35" s="89"/>
       <c r="N35" s="89"/>
       <c r="O35" s="89"/>
       <c r="P35" s="89"/>
       <c r="Q35" s="89" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="37" spans="1:24">
       <c r="G37" s="69" t="s">
+        <v>79</v>
+      </c>
+      <c r="L37" s="69" t="s">
         <v>80</v>
       </c>
-      <c r="L37" s="69" t="s">
+      <c r="Q37" s="69" t="s">
         <v>81</v>
-      </c>
-      <c r="Q37" s="69" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="38" spans="1:24">
       <c r="B38" s="69" t="s">
+        <v>82</v>
+      </c>
+      <c r="G38" t="s">
         <v>83</v>
       </c>
-      <c r="G38" t="s">
+      <c r="L38" t="s">
         <v>84</v>
       </c>
-      <c r="L38" t="s">
-        <v>85</v>
-      </c>
       <c r="Q38" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="39" spans="1:24">
       <c r="Q39" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="40" spans="1:24">
       <c r="L40" s="69" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="41" spans="1:24">
       <c r="B41" s="69" t="s">
+        <v>87</v>
+      </c>
+      <c r="G41" s="69" t="s">
+        <v>61</v>
+      </c>
+      <c r="L41" t="s">
         <v>88</v>
-      </c>
-      <c r="G41" s="69" t="s">
-        <v>62</v>
-      </c>
-      <c r="L41" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="42" spans="1:24">
       <c r="B42" t="s">
+        <v>89</v>
+      </c>
+      <c r="G42" t="s">
+        <v>62</v>
+      </c>
+      <c r="L42" t="s">
         <v>90</v>
-      </c>
-      <c r="G42" t="s">
-        <v>63</v>
-      </c>
-      <c r="L42" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="43" spans="1:24">
       <c r="B43" s="70"/>
       <c r="Q43" s="69" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="44" spans="1:24">
       <c r="G44" s="69" t="s">
+        <v>91</v>
+      </c>
+      <c r="L44" s="69" t="s">
         <v>92</v>
       </c>
-      <c r="L44" s="69" t="s">
-        <v>93</v>
-      </c>
       <c r="Q44" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="45" spans="1:24">
       <c r="Q45" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="47" spans="1:24">
       <c r="B47" s="89" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C47" s="89"/>
       <c r="D47" s="89"/>
       <c r="E47" s="89"/>
       <c r="F47" s="89"/>
       <c r="G47" s="89" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H47" s="89"/>
       <c r="I47" s="89"/>
       <c r="J47" s="89"/>
       <c r="K47" s="89"/>
       <c r="L47" s="89" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="M47" s="89"/>
       <c r="N47" s="89"/>
       <c r="O47" s="89"/>
       <c r="P47" s="89"/>
       <c r="Q47" s="89" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="48" spans="1:24">
@@ -3646,14 +3850,14 @@
       <c r="R48" s="65"/>
     </row>
     <row r="49" spans="1:24">
-      <c r="B49" t="str">
-        <v>Tel médecin</v>
+      <c r="B49" t="s">
+        <v>138</v>
       </c>
       <c r="C49" s="65"/>
       <c r="D49" s="65"/>
       <c r="G49" s="70"/>
-      <c r="L49" s="70" t="str">
-        <v>Tel ophtalmo</v>
+      <c r="L49" s="70" t="s">
+        <v>139</v>
       </c>
       <c r="R49" s="65"/>
     </row>
@@ -3708,41 +3912,41 @@
     </row>
     <row r="59" spans="1:24">
       <c r="H59" s="66"/>
-      <c r="I59" s="90" t="s">
-        <f>IF(ISBLANK(H59),"",NETWORKDAYS(TODAY(),H59,Conges!$A:$A))</f>
-        <v>19</v>
+      <c r="I59" s="90" t="str">
+        <f ca="1">IF(ISBLANK(H59),"",NETWORKDAYS(TODAY(),H59,Conges!$A:$A))</f>
+        <v/>
       </c>
       <c r="M59" s="66"/>
     </row>
     <row r="60" spans="1:24">
       <c r="H60" s="66"/>
-      <c r="I60" s="91" t="s">
-        <f>IF(ISBLANK(H60),"",NETWORKDAYS(TODAY(),H60,Conges!$B:$B))</f>
-        <v>19</v>
+      <c r="I60" s="91" t="str">
+        <f ca="1">IF(ISBLANK(H60),"",NETWORKDAYS(TODAY(),H60,Conges!$B:$B))</f>
+        <v/>
       </c>
       <c r="M60" s="66"/>
     </row>
     <row r="61" spans="1:24">
       <c r="H61" s="66"/>
-      <c r="I61" s="91" t="s">
-        <f>IF(ISBLANK(H61),"",NETWORKDAYS(TODAY(),H61,Conges!$B:$B))</f>
-        <v>19</v>
+      <c r="I61" s="91" t="str">
+        <f ca="1">IF(ISBLANK(H61),"",NETWORKDAYS(TODAY(),H61,Conges!$B:$B))</f>
+        <v/>
       </c>
       <c r="M61" s="66"/>
     </row>
     <row r="62" spans="1:24">
       <c r="H62" s="66"/>
-      <c r="I62" s="91" t="s">
-        <f>IF(ISBLANK(H62),"",NETWORKDAYS(TODAY(),H62,Conges!$A:$A))</f>
-        <v>19</v>
+      <c r="I62" s="91" t="str">
+        <f ca="1">IF(ISBLANK(H62),"",NETWORKDAYS(TODAY(),H62,Conges!$A:$A))</f>
+        <v/>
       </c>
       <c r="M62" s="66"/>
     </row>
     <row r="63" spans="1:24">
       <c r="H63" s="66"/>
-      <c r="I63" s="91" t="s">
-        <f>IF(ISBLANK(H63),"",NETWORKDAYS(TODAY(),H63,Conges!$B:$B))</f>
-        <v>19</v>
+      <c r="I63" s="91" t="str">
+        <f ca="1">IF(ISBLANK(H63),"",NETWORKDAYS(TODAY(),H63,Conges!$B:$B))</f>
+        <v/>
       </c>
       <c r="M63" s="66"/>
     </row>
@@ -3783,8 +3987,7 @@
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" selectLockedCells="1" sort="0" autoFilter="0" pivotTables="0" selectUnlockedCells="1"/>
-  <printOptions/>
   <pageMargins left="1" right="1" top="1.667" bottom="1.667" header="1" footer="1"/>
-  <pageSetup blackAndWhite="0" cellComments="asDisplayed" draft="0" errors="displayed" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="0"/>
+  <pageSetup paperSize="9" orientation="portrait" cellComments="asDisplayed"/>
 </worksheet>
 </file>
</xml_diff>